<commit_message>
feat: dump ChartModel fixture JSON
- Update dump_chart_models to extract chart objects and serialize parsed ChartModel + anchor
- Update chart_fixture_models_match to compare ChartModel JSON against parser output
- Regenerate fixtures/charts/models/* from the new schema
- Fix box-whisker fixture XML escaping so chart XML parses
- Fix fast reader workbook metadata destructuring after defined-name support
</commit_message>
<xml_diff>
--- a/fixtures/charts/xlsx/box-whisker.xlsx
+++ b/fixtures/charts/xlsx/box-whisker.xlsx
@@ -78,7 +78,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -88,8 +88,13 @@
           <a:bodyPr/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr><a:defRPr/></a:pPr>
-            <a:r><a:rPr lang="en-US"/><a:t>Box & Whisker</a:t></a:r>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Box &amp; Whisker</a:t>
+            </a:r>
           </a:p>
         </c:rich>
       </c:tx>
@@ -102,17 +107,27 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:strRef><c:f>Sheet1!$B$1</c:f></c:strRef>
+            <c:strRef>
+              <c:f>Sheet1!$B$1</c:f>
+            </c:strRef>
           </c:tx>
           <c:cat>
-            <c:strRef><c:f>Sheet1!$A$2:$A$5</c:f></c:strRef>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$5</c:f>
+            </c:strRef>
           </c:cat>
           <c:val>
-            <c:numRef><c:f>Sheet1!$B$2:$B$5</c:f></c:numRef>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$5</c:f>
+            </c:numRef>
           </c:val>
           <c:dPt>
             <c:idx val="0"/>
-            <c:spPr><a:solidFill><a:srgbClr val="FF0000"/></a:solidFill></c:spPr>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </c:spPr>
           </c:dPt>
         </c:ser>
         <c:axId val="50010001"/>
@@ -120,7 +135,9 @@
       </c:boxWhiskerChart>
       <c:catAx>
         <c:axId val="50010001"/>
-        <c:scaling><c:orientation val="minMax"/></c:scaling>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="50010002"/>
@@ -131,7 +148,9 @@
       </c:catAx>
       <c:valAx>
         <c:axId val="50010002"/>
-        <c:scaling><c:orientation val="minMax"/></c:scaling>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="0"/>
@@ -153,16 +172,14 @@
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
-
-</file>
-
-<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="UTF-8" standalone="yes"?>
+</file>
+
+<file path=xl/charts/chartEx1.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <cx:chart>
-    <cx:title>Box & Whisker</cx:title>
+    <cx:title>Box &amp; Whisker</cx:title>
   </cx:chart>
 </cx:chartSpace>
-
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>